<commit_message>
organised a bit the code, but it still needs some documentation
</commit_message>
<xml_diff>
--- a/images_information.xlsx
+++ b/images_information.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ja/GitHub/RectangularImages/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AC7F6C3-1CB6-6440-A212-8EAC01DAC344}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CAE2795-FAF3-FD46-A580-6CD2490D283C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16940" xr2:uid="{17FBEFE5-0FBC-7E4B-ADCC-FF25885A5BEF}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="76800" windowHeight="43200" xr2:uid="{17FBEFE5-0FBC-7E4B-ADCC-FF25885A5BEF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -746,8 +746,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEC6BD31-F470-1744-930F-1526590A4E21}">
   <dimension ref="A1:B116"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" zoomScale="256" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>